<commit_message>
fix: resolve failing tests
</commit_message>
<xml_diff>
--- a/cypress/fixtures/students_import/13_template.xlsx
+++ b/cypress/fixtures/students_import/13_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t xml:space="preserve">ref</t>
   </si>
@@ -46,9 +46,6 @@
     <t xml:space="preserve">Smith</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-28</t>
-  </si>
-  <si>
     <t xml:space="preserve">STD000002</t>
   </si>
   <si>
@@ -91,70 +88,52 @@
     <t xml:space="preserve">jane</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-29</t>
-  </si>
-  <si>
     <t xml:space="preserve">STD000009</t>
   </si>
   <si>
     <t xml:space="preserve">mih</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-30</t>
-  </si>
-  <si>
     <t xml:space="preserve">STD000010</t>
   </si>
   <si>
     <t xml:space="preserve">will</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-31</t>
-  </si>
-  <si>
     <t xml:space="preserve">STD000011</t>
   </si>
   <si>
     <t xml:space="preserve">jaden</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-32</t>
-  </si>
-  <si>
     <t xml:space="preserve">STD000012</t>
   </si>
   <si>
     <t xml:space="preserve">alya</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-33</t>
-  </si>
-  <si>
     <t xml:space="preserve">STD000013</t>
   </si>
   <si>
     <t xml:space="preserve">billy</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-34</t>
-  </si>
-  <si>
     <t xml:space="preserve">STD000014</t>
   </si>
   <si>
     <t xml:space="preserve">rio</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-35</t>
-  </si>
-  <si>
     <t xml:space="preserve">STD000015</t>
   </si>
   <si>
     <t xml:space="preserve">ken</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-36</t>
+    <t xml:space="preserve">STD000016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rere</t>
   </si>
 </sst>
 </file>
@@ -163,7 +142,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd\-mm\-yy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -238,20 +217,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,29 +430,29 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -487,16 +470,17 @@
         <f aca="false">CONCATENATE("user",A2,"@hei.school")</f>
         <v>userSTD000001@hei.school</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
+      <c r="E2" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -505,16 +489,17 @@
         <f aca="false">CONCATENATE("user",A3,"@hei.school")</f>
         <v>userSTD000002@hei.school</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
+      <c r="E3" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
@@ -523,16 +508,17 @@
         <f aca="false">CONCATENATE("user",A4,"@hei.school")</f>
         <v>userSTD000003@hei.school</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
+      <c r="E4" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -541,16 +527,17 @@
         <f aca="false">CONCATENATE("user",A5,"@hei.school")</f>
         <v>userSTD000004@hei.school</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
+      <c r="E5" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -559,16 +546,17 @@
         <f aca="false">CONCATENATE("user",A6,"@hei.school")</f>
         <v>userSTD000005@hei.school</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
+      <c r="E6" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -577,16 +565,17 @@
         <f aca="false">CONCATENATE("user",A7,"@hei.school")</f>
         <v>userSTD000006@hei.school</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>8</v>
+      <c r="E7" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -595,16 +584,17 @@
         <f aca="false">CONCATENATE("user",A8,"@hei.school")</f>
         <v>userSTD000007@hei.school</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>8</v>
+      <c r="E8" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -613,16 +603,17 @@
         <f aca="false">CONCATENATE("user",A9,"@hei.school")</f>
         <v>userSTD000003@hei.school</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>8</v>
+      <c r="E9" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -631,16 +622,17 @@
         <f aca="false">CONCATENATE("user",A10,"@hei.school")</f>
         <v>userSTD000004@hei.school</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>8</v>
+      <c r="E10" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
@@ -649,16 +641,17 @@
         <f aca="false">CONCATENATE("user",A11,"@hei.school")</f>
         <v>userSTD000005@hei.school</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>8</v>
+      <c r="E11" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>7</v>
@@ -667,16 +660,17 @@
         <f aca="false">CONCATENATE("user",A12,"@hei.school")</f>
         <v>userSTD000006@hei.school</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>8</v>
+      <c r="E12" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>7</v>
@@ -685,16 +679,17 @@
         <f aca="false">CONCATENATE("user",A13,"@hei.school")</f>
         <v>userSTD000007@hei.school</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>8</v>
+      <c r="E13" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
@@ -703,16 +698,17 @@
         <f aca="false">CONCATENATE("user",A14,"@hei.school")</f>
         <v>userSTD000008@hei.school</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>23</v>
+      <c r="E14" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>7</v>
@@ -721,16 +717,17 @@
         <f aca="false">CONCATENATE("user",A15,"@hei.school")</f>
         <v>userSTD000009@hei.school</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>26</v>
+      <c r="E15" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>7</v>
@@ -739,16 +736,17 @@
         <f aca="false">CONCATENATE("user",A16,"@hei.school")</f>
         <v>userSTD000010@hei.school</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>29</v>
+      <c r="E16" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>7</v>
@@ -757,16 +755,17 @@
         <f aca="false">CONCATENATE("user",A17,"@hei.school")</f>
         <v>userSTD000011@hei.school</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>32</v>
+      <c r="E17" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>7</v>
@@ -775,16 +774,17 @@
         <f aca="false">CONCATENATE("user",A18,"@hei.school")</f>
         <v>userSTD000012@hei.school</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>35</v>
+      <c r="E18" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>7</v>
@@ -793,16 +793,17 @@
         <f aca="false">CONCATENATE("user",A19,"@hei.school")</f>
         <v>userSTD000013@hei.school</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>38</v>
+      <c r="E19" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
@@ -811,16 +812,17 @@
         <f aca="false">CONCATENATE("user",A20,"@hei.school")</f>
         <v>userSTD000014@hei.school</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>41</v>
+      <c r="E20" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>7</v>
@@ -829,11 +831,30 @@
         <f aca="false">CONCATENATE("user",A21,"@hei.school")</f>
         <v>userSTD000015@hei.school</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="E21" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f aca="false">CONCATENATE("user",A22,"@hei.school")</f>
+        <v>userSTD000016@hei.school</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45584</v>
+      </c>
+    </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>